<commit_message>
correct wood reuse factors and documentation
</commit_message>
<xml_diff>
--- a/impactFactors/intermediate/importedButUnalteredForCheckingVsGabi.xlsx
+++ b/impactFactors/intermediate/importedButUnalteredForCheckingVsGabi.xlsx
@@ -36007,7 +36007,7 @@
         <v>68</v>
       </c>
       <c r="G1383" t="n">
-        <v>-268.735329279232</v>
+        <v>-2406.05391514515</v>
       </c>
       <c r="H1383" t="s">
         <v>69</v>
@@ -50151,7 +50151,7 @@
         <v>68</v>
       </c>
       <c r="G1927" t="n">
-        <v>-459.081135398217</v>
+        <v>-2596.39972126413</v>
       </c>
       <c r="H1927" t="s">
         <v>71</v>
@@ -50203,7 +50203,7 @@
         <v>68</v>
       </c>
       <c r="G1929" t="n">
-        <v>503.464817609131</v>
+        <v>-1633.85376825679</v>
       </c>
       <c r="H1929" t="s">
         <v>71</v>
@@ -57769,7 +57769,7 @@
         <v>68</v>
       </c>
       <c r="G2220" t="n">
-        <v>-306.889839616597</v>
+        <v>-2444.20842548251</v>
       </c>
       <c r="H2220" t="s">
         <v>74</v>
@@ -71913,7 +71913,7 @@
         <v>68</v>
       </c>
       <c r="G2764" t="n">
-        <v>-497.298289769922</v>
+        <v>-2634.61687563584</v>
       </c>
       <c r="H2764" t="s">
         <v>76</v>
@@ -71965,7 +71965,7 @@
         <v>68</v>
       </c>
       <c r="G2766" t="n">
-        <v>465.247663237425</v>
+        <v>-1672.07092262849</v>
       </c>
       <c r="H2766" t="s">
         <v>76</v>

</xml_diff>

<commit_message>
correct (even more) wood impact factors
</commit_message>
<xml_diff>
--- a/impactFactors/intermediate/importedButUnalteredForCheckingVsGabi.xlsx
+++ b/impactFactors/intermediate/importedButUnalteredForCheckingVsGabi.xlsx
@@ -30885,7 +30885,7 @@
         <v>68</v>
       </c>
       <c r="G1186" t="n">
-        <v>-20.7582203170089</v>
+        <v>51.8173035875543</v>
       </c>
       <c r="H1186" t="s">
         <v>69</v>
@@ -30937,7 +30937,7 @@
         <v>68</v>
       </c>
       <c r="G1188" t="n">
-        <v>-28.3439736869297</v>
+        <v>80.5193121699151</v>
       </c>
       <c r="H1188" t="s">
         <v>69</v>
@@ -35799,7 +35799,7 @@
         <v>68</v>
       </c>
       <c r="G1375" t="n">
-        <v>-28.3439736869297</v>
+        <v>80.5193121699151</v>
       </c>
       <c r="H1375" t="s">
         <v>69</v>
@@ -36007,7 +36007,7 @@
         <v>68</v>
       </c>
       <c r="G1383" t="n">
-        <v>-2406.05391514515</v>
+        <v>-268.735329279232</v>
       </c>
       <c r="H1383" t="s">
         <v>69</v>
@@ -36059,7 +36059,7 @@
         <v>68</v>
       </c>
       <c r="G1385" t="n">
-        <v>-20.7582203170089</v>
+        <v>51.8173035875543</v>
       </c>
       <c r="H1385" t="s">
         <v>69</v>
@@ -36111,7 +36111,7 @@
         <v>68</v>
       </c>
       <c r="G1387" t="n">
-        <v>-28.3439736869297</v>
+        <v>80.5193121699151</v>
       </c>
       <c r="H1387" t="s">
         <v>69</v>
@@ -52647,7 +52647,7 @@
         <v>68</v>
       </c>
       <c r="G2023" t="n">
-        <v>56.8686961921398</v>
+        <v>129.444220096703</v>
       </c>
       <c r="H2023" t="s">
         <v>74</v>
@@ -52699,7 +52699,7 @@
         <v>68</v>
       </c>
       <c r="G2025" t="n">
-        <v>12.154469273813</v>
+        <v>121.017755130658</v>
       </c>
       <c r="H2025" t="s">
         <v>74</v>
@@ -57561,7 +57561,7 @@
         <v>68</v>
       </c>
       <c r="G2212" t="n">
-        <v>12.154469273813</v>
+        <v>121.017755130658</v>
       </c>
       <c r="H2212" t="s">
         <v>74</v>
@@ -57769,7 +57769,7 @@
         <v>68</v>
       </c>
       <c r="G2220" t="n">
-        <v>-2444.20842548251</v>
+        <v>-306.889839616597</v>
       </c>
       <c r="H2220" t="s">
         <v>74</v>
@@ -57821,7 +57821,7 @@
         <v>68</v>
       </c>
       <c r="G2222" t="n">
-        <v>56.8686961921398</v>
+        <v>129.444220096703</v>
       </c>
       <c r="H2222" t="s">
         <v>74</v>
@@ -57873,7 +57873,7 @@
         <v>68</v>
       </c>
       <c r="G2224" t="n">
-        <v>12.154469273813</v>
+        <v>121.017755130658</v>
       </c>
       <c r="H2224" t="s">
         <v>74</v>

</xml_diff>